<commit_message>
adding to HJ7 collections and updates for Dec. 20/22
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-8-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-8-occ-entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF874A5-1EBD-BB49-859D-F45EC00BC356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2698643E-2D46-E14F-8064-B4EADAB81069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -4204,7 +4204,7 @@
   <dimension ref="A1:AF215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="H219" sqref="H219"/>
     </sheetView>

</xml_diff>